<commit_message>
AutoExerciseTest day03_ Practice ders sonu
</commit_message>
<xml_diff>
--- a/src/test/java/day12_webtables_excel/ulkeler.xlsx
+++ b/src/test/java/day12_webtables_excel/ulkeler.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68D1A50-D932-4B32-9800-BBC0BE1CCF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15E1BD5-B8DC-45FE-8180-B281E453C6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="1530" windowWidth="17055" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="578">
   <si>
     <t>Ülke (İngilizce)</t>
   </si>
@@ -1778,17 +1778,19 @@
     </r>
   </si>
   <si>
-    <t>NUFUS</t>
-  </si>
-  <si>
-    <t>1000000</t>
+    <t>Nufus</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>3000000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2238,13 +2240,13 @@
   <dimension ref="A1:F191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:D17"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="36.28515625" collapsed="false"/>
+    <col min="1" max="4" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2352,6 +2354,12 @@
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>577</v>
+      </c>
+      <c r="F7" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>